<commit_message>
code quality index finished
</commit_message>
<xml_diff>
--- a/files/Regelwerk.xlsx
+++ b/files/Regelwerk.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="838">
   <si>
     <t>Classification</t>
   </si>
@@ -2553,6 +2553,9 @@
   </si>
   <si>
     <t>19 Regelkomplexe  / Einzelregeln für Lehrveranstaltung equivalent zum SWP-Code-Quality-Index - 3 blocker, 6 critical, 3 major, 6 minor, 1 info</t>
+  </si>
+  <si>
+    <t>Literal suffixes should not be upper case</t>
   </si>
 </sst>
 </file>
@@ -3037,7 +3040,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3083,9 +3086,11 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="19"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="17" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3095,7 +3100,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10479,19 +10483,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>647</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
@@ -11611,19 +11615,19 @@
     </row>
     <row r="50" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="46" t="s">
         <v>648</v>
       </c>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
-      <c r="J51" s="45"/>
-      <c r="K51" s="45"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
@@ -12496,19 +12500,19 @@
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A90" s="45" t="s">
+      <c r="A90" s="46" t="s">
         <v>649</v>
       </c>
-      <c r="B90" s="45"/>
-      <c r="C90" s="45"/>
-      <c r="D90" s="45"/>
-      <c r="E90" s="45"/>
-      <c r="F90" s="45"/>
-      <c r="G90" s="45"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="45"/>
-      <c r="J90" s="45"/>
-      <c r="K90" s="45"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="46"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="46"/>
+      <c r="G90" s="46"/>
+      <c r="H90" s="46"/>
+      <c r="I90" s="46"/>
+      <c r="J90" s="46"/>
+      <c r="K90" s="46"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="35" t="s">
@@ -12844,11 +12848,11 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="46" t="s">
         <v>799</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
@@ -15043,23 +15047,23 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="46" t="s">
+      <c r="A109" s="48" t="s">
         <v>812</v>
       </c>
-      <c r="B109" s="46"/>
-      <c r="C109" s="46"/>
-      <c r="D109" s="46"/>
-      <c r="E109" s="46"/>
-      <c r="F109" s="46"/>
+      <c r="B109" s="48"/>
+      <c r="C109" s="48"/>
+      <c r="D109" s="48"/>
+      <c r="E109" s="48"/>
+      <c r="F109" s="48"/>
       <c r="G109" s="35"/>
     </row>
     <row r="110" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="49"/>
-      <c r="B110" s="49"/>
-      <c r="C110" s="49"/>
-      <c r="D110" s="49"/>
-      <c r="E110" s="49"/>
-      <c r="F110" s="49"/>
+      <c r="A110" s="47"/>
+      <c r="B110" s="47"/>
+      <c r="C110" s="47"/>
+      <c r="D110" s="47"/>
+      <c r="E110" s="47"/>
+      <c r="F110" s="47"/>
       <c r="G110" s="35"/>
     </row>
   </sheetData>
@@ -15103,20 +15107,20 @@
       <c r="A1" s="44" t="s">
         <v>717</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>729</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46" t="s">
         <v>728</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
       <c r="L1" s="44" t="s">
         <v>731</v>
       </c>
@@ -16055,54 +16059,54 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="46" t="s">
         <v>757</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="50" t="s">
         <v>758</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="50" t="s">
         <v>759</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="50" t="s">
         <v>793</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="49" t="s">
         <v>760</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -16124,15 +16128,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="80.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="74.5546875" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" customWidth="1"/>
     <col min="4" max="4" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16538,8 +16542,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="35" t="s">
-        <v>528</v>
+      <c r="B41" s="45" t="s">
+        <v>837</v>
       </c>
       <c r="C41" t="s">
         <v>675</v>
@@ -16814,16 +16818,16 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B69" s="45" t="s">
+      <c r="B69" s="46" t="s">
         <v>812</v>
       </c>
-      <c r="C69" s="45"/>
+      <c r="C69" s="46"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B70" s="45" t="s">
+      <c r="B70" s="46" t="s">
         <v>836</v>
       </c>
-      <c r="C70" s="45"/>
+      <c r="C70" s="46"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="35"/>

</xml_diff>